<commit_message>
Assembled options for the prfTimeShift
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/submitGears/AssemblePRFModelOpts.xlsx
+++ b/code/submitGears/AssemblePRFModelOpts.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="28020" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="11500" yWindow="2800" windowWidth="21780" windowHeight="13040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Untitled" localSheetId="0">Sheet1!$B$4:$D$44</definedName>
+    <definedName name="Untitled" localSheetId="0">Sheet1!$B$5:$D$45</definedName>
+    <definedName name="Untitled_1" localSheetId="0">Sheet1!$F$5:$G$46</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,10 +33,19 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="Untitled" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/aguirre/Desktop/Untitled.txt" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="/Users/aguirre/Desktop/Untitled.txt" space="1" consecutive="1">
       <textFields count="5">
         <textField/>
         <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="Untitled1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/aguirre/Desktop/Untitled.txt" space="1" consecutive="1">
+      <textFields count="3">
         <textField/>
         <textField/>
         <textField/>
@@ -46,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="146">
   <si>
     <t>TOME_3001</t>
   </si>
@@ -208,6 +218,282 @@
   </si>
   <si>
     <t>Calculated Nov 3, 2019</t>
+  </si>
+  <si>
+    <t>TOME_3001_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8562,0.1350,-0.2175]</t>
+  </si>
+  <si>
+    <t>TOME_3002_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7937,-0.5338,-0.2704]</t>
+  </si>
+  <si>
+    <t>TOME_3003_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8501,-0.0683,-0.0515]</t>
+  </si>
+  <si>
+    <t>TOME_3004_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8111,-0.4550,-0.2459]</t>
+  </si>
+  <si>
+    <t>TOME_3005_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8334,-0.2640,-0.2553]</t>
+  </si>
+  <si>
+    <t>TOME_3007_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8235,-0.2968,-0.2871]</t>
+  </si>
+  <si>
+    <t>TOME_3008_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8496,-0.1993,-0.0990]</t>
+  </si>
+  <si>
+    <t>TOME_3009_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8475,0.0050,-0.2745]</t>
+  </si>
+  <si>
+    <t>TOME_3011_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8248,-0.3922,-0.0841]</t>
+  </si>
+  <si>
+    <t>TOME_3012_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8522,0.0015,0.0018]</t>
+  </si>
+  <si>
+    <t>TOME_3013_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8234,-0.4302,-0.2296]</t>
+  </si>
+  <si>
+    <t>TOME_3014_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8393,-0.3596,-0.1444]</t>
+  </si>
+  <si>
+    <t>TOME_3015_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8292,-0.3717,-0.2394]</t>
+  </si>
+  <si>
+    <t>TOME_3016_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7720,-0.4753,-0.3207]</t>
+  </si>
+  <si>
+    <t>TOME_3018_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7369,-0.7276,-0.3476]</t>
+  </si>
+  <si>
+    <t>TOME_3019_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8285,-0.4219,-0.1944]</t>
+  </si>
+  <si>
+    <t>TOME_3020_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8572,0.2510,-0.1770]</t>
+  </si>
+  <si>
+    <t>TOME_3021_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7413,-0.4155,-0.3692]</t>
+  </si>
+  <si>
+    <t>TOME_3022_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8546,-0.0210,-0.1566]</t>
+  </si>
+  <si>
+    <t>TOME_3023_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8429,-0.3122,-0.2306]</t>
+  </si>
+  <si>
+    <t>TOME_3024_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8142,-0.4811,-0.1048]</t>
+  </si>
+  <si>
+    <t>TOME_3025_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7424,-0.4278,-0.3539]</t>
+  </si>
+  <si>
+    <t>TOME_3026_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8516,-0.0032,-0.2694]</t>
+  </si>
+  <si>
+    <t>TOME_3028_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8320,-0.0692,-0.2544]</t>
+  </si>
+  <si>
+    <t>TOME_3029_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8178,-0.3931,-0.2711]</t>
+  </si>
+  <si>
+    <t>TOME_3030_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8145,-0.0536,-0.3228]</t>
+  </si>
+  <si>
+    <t>TOME_3031_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7265,-0.5069,-0.3527]</t>
+  </si>
+  <si>
+    <t>TOME_3032_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8519,0.1765,-0.1441]</t>
+  </si>
+  <si>
+    <t>TOME_3033_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8373,-0.3324,-0.2508]</t>
+  </si>
+  <si>
+    <t>TOME_3034_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7800,-0.3337,-0.3357]</t>
+  </si>
+  <si>
+    <t>TOME_3035_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7919,-0.1690,-0.3364]</t>
+  </si>
+  <si>
+    <t>TOME_3036_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8046,-0.1832,-0.2215]</t>
+  </si>
+  <si>
+    <t>TOME_3037_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7476,-0.7178,-0.3492]</t>
+  </si>
+  <si>
+    <t>TOME_3038_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.6976,-1.0396,-0.3401]</t>
+  </si>
+  <si>
+    <t>TOME_3039_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7270,-0.7492,-0.3650]</t>
+  </si>
+  <si>
+    <t>TOME_3040_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8276,-0.4072,-0.2490]</t>
+  </si>
+  <si>
+    <t>TOME_3042_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7255,-0.5331,-0.3660]</t>
+  </si>
+  <si>
+    <t>TOME_3043_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7662,-0.6241,-0.3333]</t>
+  </si>
+  <si>
+    <t>TOME_3044_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7537,-1.0196,-0.2191]</t>
+  </si>
+  <si>
+    <t>TOME_3045_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8295,-0.3232,-0.2605]</t>
+  </si>
+  <si>
+    <t>TOME_3046_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.7811,-0.9330,-0.1807]</t>
+  </si>
+  <si>
+    <t>TOME_3046</t>
+  </si>
+  <si>
+    <t>HRF params from flobsHRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculated Nov 3, 2019, using </t>
+  </si>
+  <si>
+    <t>SCRIPT_calcMagnification.m</t>
+  </si>
+  <si>
+    <t>extractHRFParams.m</t>
+  </si>
+  <si>
+    <t>Assembled modelOpts</t>
+  </si>
+  <si>
+    <t>Check ID match</t>
+  </si>
+  <si>
+    <t>(XXX means mismatch)</t>
+  </si>
+  <si>
+    <t>TOME_3017_flobsHRF_results.mat</t>
+  </si>
+  <si>
+    <t>(hrfParams),[0.8077,-0.4303,-0.2938]</t>
   </si>
 </sst>
 </file>
@@ -243,8 +529,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -260,6 +549,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Untitled_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Untitled" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -526,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D44"/>
+  <dimension ref="B1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="H31" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,9 +830,10 @@
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>50</v>
       </c>
@@ -549,461 +843,1086 @@
       <c r="D1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="F2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>81916</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f>IF(B5=LEFT(F5,9),"","XXX")</f>
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <f>CONCATENATE("'","(pixelsPerDegree),5.1751,(polyDeg),5,",D5,",",G5,"'")</f>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.98,(hrfParams),[0.8562,0.1350,-0.2175]'</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>82616</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" ref="K6:K46" si="0">IF(B6=LEFT(F6,9),"","XXX")</f>
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" ref="M6:M46" si="1">CONCATENATE("'","(pixelsPerDegree),5.1751,(polyDeg),5,",D6,",",G6,"'")</f>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.7937,-0.5338,-0.2704]'</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>91616</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.87,(hrfParams),[0.8501,-0.0683,-0.0515]'</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>101416</v>
       </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8111,-0.4550,-0.2459]'</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>100316</v>
       </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8334,-0.2640,-0.2553]'</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>101716</v>
       </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8235,-0.2968,-0.2871]'</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>103116</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.94,(hrfParams),[0.8496,-0.1993,-0.0990]'</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>102516</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.95,(hrfParams),[0.8475,0.0050,-0.2745]'</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>12017</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.8248,-0.3922,-0.0841]'</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>20317</v>
       </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8522,0.0015,0.0018]'</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>11117</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.94,(hrfParams),[0.8234,-0.4302,-0.2296]'</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>21717</v>
       </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8393,-0.3596,-0.1444]'</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>32417</v>
       </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8292,-0.3717,-0.2394]'</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>32017</v>
       </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" t="s">
+        <v>81</v>
+      </c>
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7720,-0.4753,-0.3207]'</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>33117</v>
       </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>144</v>
+      </c>
+      <c r="G19" t="s">
+        <v>145</v>
+      </c>
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8077,-0.4303,-0.2938]'</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>51217</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
+        <v>83</v>
+      </c>
+      <c r="K20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.97,(hrfParams),[0.7369,-0.7276,-0.3476]'</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>50317</v>
       </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" t="s">
+        <v>85</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8285,-0.4219,-0.1944]'</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>50517</v>
       </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" t="s">
+        <v>87</v>
+      </c>
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8572,0.2510,-0.1770]'</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>60917</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="s">
+        <v>89</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.7413,-0.4155,-0.3692]'</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>61617</v>
       </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" t="s">
+        <v>91</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8546,-0.0210,-0.1566]'</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>81117</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="F25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.95,(hrfParams),[0.8429,-0.3122,-0.2306]'</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>90817</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="F26" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" t="s">
+        <v>95</v>
+      </c>
+      <c r="K26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.8142,-0.4811,-0.1048]'</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>91517</v>
       </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" t="s">
+        <v>97</v>
+      </c>
+      <c r="K27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7424,-0.4278,-0.3539]'</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>100617</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+      <c r="F28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" t="s">
+        <v>99</v>
+      </c>
+      <c r="K28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.8516,-0.0032,-0.2694]'</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>111517</v>
       </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" t="s">
+        <v>101</v>
+      </c>
+      <c r="K29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8320,-0.0692,-0.2544]'</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>120617</v>
       </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" t="s">
+        <v>103</v>
+      </c>
+      <c r="K30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8178,-0.3931,-0.2711]'</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>11018</v>
       </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>104</v>
+      </c>
+      <c r="G31" t="s">
+        <v>105</v>
+      </c>
+      <c r="K31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8145,-0.0536,-0.3228]'</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>90718</v>
       </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" t="s">
+        <v>107</v>
+      </c>
+      <c r="K32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7265,-0.5069,-0.3527]'</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>22818</v>
       </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>108</v>
+      </c>
+      <c r="G33" t="s">
+        <v>109</v>
+      </c>
+      <c r="K33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8519,0.1765,-0.1441]'</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>41318</v>
       </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" t="s">
+        <v>111</v>
+      </c>
+      <c r="K34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8373,-0.3324,-0.2508]'</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>62218</v>
       </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>112</v>
+      </c>
+      <c r="G35" t="s">
+        <v>113</v>
+      </c>
+      <c r="K35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7800,-0.3337,-0.3357]'</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>52518</v>
       </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" t="s">
+        <v>115</v>
+      </c>
+      <c r="K36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7919,-0.1690,-0.3364]'</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>62218</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+      <c r="F37" t="s">
+        <v>116</v>
+      </c>
+      <c r="G37" t="s">
+        <v>117</v>
+      </c>
+      <c r="K37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.8046,-0.1832,-0.2215]'</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>72518</v>
       </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>118</v>
+      </c>
+      <c r="G38" t="s">
+        <v>119</v>
+      </c>
+      <c r="K38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7476,-0.7178,-0.3492]'</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>73118</v>
       </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>120</v>
+      </c>
+      <c r="G39" t="s">
+        <v>121</v>
+      </c>
+      <c r="K39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.6976,-1.0396,-0.3401]'</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>43</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>82218</v>
       </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
+        <v>122</v>
+      </c>
+      <c r="G40" t="s">
+        <v>123</v>
+      </c>
+      <c r="K40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7270,-0.7492,-0.3650]'</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>44</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>92818</v>
       </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>124</v>
+      </c>
+      <c r="G41" t="s">
+        <v>125</v>
+      </c>
+      <c r="K41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8276,-0.4072,-0.2490]'</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>81618</v>
       </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>126</v>
+      </c>
+      <c r="G42" t="s">
+        <v>127</v>
+      </c>
+      <c r="K42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7255,-0.5331,-0.3660]'</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>46</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>100218</v>
       </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>128</v>
+      </c>
+      <c r="G43" t="s">
+        <v>129</v>
+      </c>
+      <c r="K43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7662,-0.6241,-0.3333]'</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
         <v>47</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>111718</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+      <c r="F44" t="s">
+        <v>130</v>
+      </c>
+      <c r="G44" t="s">
+        <v>131</v>
+      </c>
+      <c r="K44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.7537,-1.0196,-0.2191]'</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>48</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>42619</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>49</v>
+      </c>
+      <c r="F45" t="s">
+        <v>132</v>
+      </c>
+      <c r="G45" t="s">
+        <v>133</v>
+      </c>
+      <c r="K45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.90,(hrfParams),[0.8295,-0.3232,-0.2605]'</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46">
+        <v>91419</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+      <c r="F46" t="s">
+        <v>134</v>
+      </c>
+      <c r="G46" t="s">
+        <v>135</v>
+      </c>
+      <c r="K46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" si="1"/>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.90,(hrfParams),[0.7811,-0.9330,-0.1807]'</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the screen magnification values
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/submitGears/AssemblePRFModelOpts.xlsx
+++ b/code/submitGears/AssemblePRFModelOpts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11500" yWindow="2800" windowWidth="21780" windowHeight="13040" tabRatio="500"/>
+    <workbookView xWindow="7020" yWindow="2800" windowWidth="21780" windowHeight="13040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="Untitled" localSheetId="0">Sheet1!$B$5:$D$45</definedName>
     <definedName name="Untitled_1" localSheetId="0">Sheet1!$F$5:$G$46</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -44,7 +44,7 @@
     </textPr>
   </connection>
   <connection id="2" name="Untitled1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/aguirre/Desktop/Untitled.txt" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="/Users/aguirre/Desktop/Untitled.txt" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="145">
   <si>
     <t>TOME_3001</t>
   </si>
@@ -73,9 +73,6 @@
     <t>TOME_3003</t>
   </si>
   <si>
-    <t>(screenMagnification),0.87</t>
-  </si>
-  <si>
     <t>TOME_3004</t>
   </si>
   <si>
@@ -91,15 +88,9 @@
     <t>TOME_3008</t>
   </si>
   <si>
-    <t>(screenMagnification),0.94</t>
-  </si>
-  <si>
     <t>TOME_3009</t>
   </si>
   <si>
-    <t>(screenMagnification),0.95</t>
-  </si>
-  <si>
     <t>TOME_3011</t>
   </si>
   <si>
@@ -205,9 +196,6 @@
     <t>TOME_3045</t>
   </si>
   <si>
-    <t>(screenMagnification),0.90</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -494,6 +482,15 @@
   </si>
   <si>
     <t>(hrfParams),[0.8077,-0.4303,-0.2938]</t>
+  </si>
+  <si>
+    <t>(screenMagnification),0.89</t>
+  </si>
+  <si>
+    <t>(screenMagnification),0.91</t>
+  </si>
+  <si>
+    <t>(screenMagnification),0.92</t>
   </si>
 </sst>
 </file>
@@ -821,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="H31" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5:M46"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,44 +832,44 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="M3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
@@ -883,13 +880,13 @@
         <v>81916</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="K5" s="1" t="str">
         <f>IF(B5=LEFT(F5,9),"","XXX")</f>
@@ -897,7 +894,7 @@
       </c>
       <c r="M5" t="str">
         <f>CONCATENATE("'","(pixelsPerDegree),5.1751,(polyDeg),5,",D5,",",G5,"'")</f>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.98,(hrfParams),[0.8562,0.1350,-0.2175]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.8562,0.1350,-0.2175]'</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
@@ -908,13 +905,13 @@
         <v>82616</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K6" s="1" t="str">
         <f t="shared" ref="K6:K46" si="0">IF(B6=LEFT(F6,9),"","XXX")</f>
@@ -922,7 +919,7 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" ref="M6:M46" si="1">CONCATENATE("'","(pixelsPerDegree),5.1751,(polyDeg),5,",D6,",",G6,"'")</f>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.7937,-0.5338,-0.2704]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.7937,-0.5338,-0.2704]'</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
@@ -933,13 +930,13 @@
         <v>91616</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -947,24 +944,24 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.87,(hrfParams),[0.8501,-0.0683,-0.0515]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.89,(hrfParams),[0.8501,-0.0683,-0.0515]'</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>101416</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -977,19 +974,19 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>100316</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1002,19 +999,19 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>101716</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1027,19 +1024,19 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>103116</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1047,24 +1044,24 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.94,(hrfParams),[0.8496,-0.1993,-0.0990]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.98,(hrfParams),[0.8496,-0.1993,-0.0990]'</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>102516</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1072,24 +1069,24 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.95,(hrfParams),[0.8475,0.0050,-0.2745]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.8475,0.0050,-0.2745]'</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>12017</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1097,24 +1094,24 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.8248,-0.3922,-0.0841]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.8248,-0.3922,-0.0841]'</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>20317</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1127,19 +1124,19 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>11117</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1147,24 +1144,24 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.94,(hrfParams),[0.8234,-0.4302,-0.2296]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.98,(hrfParams),[0.8234,-0.4302,-0.2296]'</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>21717</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1177,19 +1174,19 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>32417</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1202,19 +1199,19 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>32017</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1227,19 +1224,19 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>33117</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G19" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="K19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1252,19 +1249,19 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>51217</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="K20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1277,19 +1274,19 @@
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>50317</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1302,19 +1299,19 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>50517</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1327,19 +1324,19 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>60917</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1347,24 +1344,24 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.7413,-0.4155,-0.3692]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.7413,-0.4155,-0.3692]'</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>61617</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1377,19 +1374,19 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>81117</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="K25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1397,24 +1394,24 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.95,(hrfParams),[0.8429,-0.3122,-0.2306]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.98,(hrfParams),[0.8429,-0.3122,-0.2306]'</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>90817</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G26" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1422,24 +1419,24 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.8142,-0.4811,-0.1048]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),1.00,(hrfParams),[0.8142,-0.4811,-0.1048]'</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>91517</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1452,19 +1449,19 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C28">
         <v>100617</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1472,24 +1469,24 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.8516,-0.0032,-0.2694]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.8516,-0.0032,-0.2694]'</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C29">
         <v>111517</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G29" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1502,19 +1499,19 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <v>120617</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1527,19 +1524,19 @@
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>11018</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G31" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1552,19 +1549,19 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>90718</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="K32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1577,19 +1574,19 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C33">
         <v>22818</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K33" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1602,19 +1599,19 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C34">
         <v>41318</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1627,19 +1624,19 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>62218</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G35" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1652,19 +1649,19 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C36">
         <v>52518</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G36" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K36" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1677,19 +1674,19 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>62218</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G37" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="K37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1697,24 +1694,24 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.8046,-0.1832,-0.2215]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.8046,-0.1832,-0.2215]'</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C38">
         <v>72518</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1727,19 +1724,19 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C39">
         <v>73118</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G39" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K39" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1752,19 +1749,19 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C40">
         <v>82218</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K40" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1777,19 +1774,19 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C41">
         <v>92818</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G41" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1802,19 +1799,19 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C42">
         <v>81618</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G42" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K42" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1827,19 +1824,19 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C43">
         <v>100218</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G43" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K43" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1852,19 +1849,19 @@
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C44">
         <v>111718</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F44" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G44" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K44" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1872,24 +1869,24 @@
       </c>
       <c r="M44" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.96,(hrfParams),[0.7537,-1.0196,-0.2191]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.99,(hrfParams),[0.7537,-1.0196,-0.2191]'</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C45">
         <v>42619</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="F45" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K45" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1897,24 +1894,24 @@
       </c>
       <c r="M45" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.90,(hrfParams),[0.8295,-0.3232,-0.2605]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.91,(hrfParams),[0.8295,-0.3232,-0.2605]'</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C46">
         <v>91419</v>
       </c>
       <c r="D46" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="F46" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G46" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K46" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1922,7 +1919,7 @@
       </c>
       <c r="M46" t="str">
         <f t="shared" si="1"/>
-        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.90,(hrfParams),[0.7811,-0.9330,-0.1807]'</v>
+        <v>'(pixelsPerDegree),5.1751,(polyDeg),5,(screenMagnification),0.92,(hrfParams),[0.7811,-0.9330,-0.1807]'</v>
       </c>
     </row>
   </sheetData>

</xml_diff>